<commit_message>
Added single and single_page mode to ART
</commit_message>
<xml_diff>
--- a/data_raw/dicts/ART_dict.xlsx
+++ b/data_raw/dicts/ART_dict.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2EEAFC-F7CA-46B9-9813-B90A6FA162ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2975DEE7-7D76-4B78-8629-6DEB91913537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SRS_dict" sheetId="1" r:id="rId1"/>
+    <sheet name="ART_dict" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>key</t>
   </si>
@@ -124,15 +124,6 @@
     <t>Artist Recognition Test</t>
   </si>
   <si>
-    <t>Sie werden nun mehrere Paare von Namen sehen und müssen jeweils entscheiden, welcher der Persoen ein Literat (Dichter/Schriftsteller) ist.</t>
-  </si>
-  <si>
-    <t>Welcher der Personen ist ein Literat ?&lt;br/&gt; Klicken Sie auf den Namen, sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
-  </si>
-  <si>
-    <t>Who of the persons is a literary writer? &lt;br/&gt; Click on the name, you have {{time_out}} seconds time.</t>
-  </si>
-  <si>
     <t>Willkommen zum Literatenquiz!</t>
   </si>
   <si>
@@ -158,6 +149,60 @@
   </si>
   <si>
     <t>You answered {{num_correct}} out of {{num_items}} questions correctly ({{perc_correct}}%).</t>
+  </si>
+  <si>
+    <t>PROMPT_SINGLE_PAGE</t>
+  </si>
+  <si>
+    <t>Bitte wählen Sie alle Literat:innen (Dichter:innen, Romanautor:innen, Dramatiker:innen)  aus der untenstehenden Liste aus.  Sie haben {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>FEEDBACK_SINGLE_PAGE</t>
+  </si>
+  <si>
+    <t>Please select all literary writers (poets, novelists, playwrights). You have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>Who of the persons is a literary writer? &lt;br/&gt; Click on the name, you have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>Sie haben {{num_correct}} Literaten aus {{num_items}} Namen richtig erkannt ({{perc_correct}}%, Punkte: {{points}}).</t>
+  </si>
+  <si>
+    <t>You answered {{num_correct}} out of {{num_items}} questions correctly ({{perc_correct}}%,  Points: {{points}}).</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>PROMPT_SINGLE</t>
+  </si>
+  <si>
+    <t>Ist &lt;b&gt;{{name}}&lt;/b&gt; eine Literat:in?&lt;br/&gt; Klicken Sie Ja oder Nein, sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
+  </si>
+  <si>
+    <t>Welcher der Personen ist eine Literat:in?&lt;br/&gt; Klicken Sie auf den Namen, sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
+  </si>
+  <si>
+    <t>Sie werden nun mehrere Paare von Namen sehen und müssen jeweils entscheiden, welcher der Persoen eine Literatin (Dichter:in, Schriftsteller:in, Dramatiker:in) ist.</t>
+  </si>
+  <si>
+    <t>Is &lt;b&gt;{{name}}&lt;/b&gt; a literary writer? &lt;br/&gt; Click Yes or No, you have {{time_out}} seconds.</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,10 +1074,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -1043,10 +1088,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1054,142 +1099,197 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added two new modes to ART (single and single_page).
</commit_message>
<xml_diff>
--- a/data_raw/dicts/ART_dict.xlsx
+++ b/data_raw/dicts/ART_dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2975DEE7-7D76-4B78-8629-6DEB91913537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA30C93-CCC2-4390-ACCE-A2C82C1AB252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>key</t>
   </si>
@@ -31,12 +31,6 @@
     <t>en</t>
   </si>
   <si>
-    <t>INSTRUCTIONS</t>
-  </si>
-  <si>
-    <t>PROMPT</t>
-  </si>
-  <si>
     <t>EXAMPLE_HEADER</t>
   </si>
   <si>
@@ -52,75 +46,15 @@
     <t>WELCOME</t>
   </si>
   <si>
-    <t>PRACTICE_ITEMS</t>
-  </si>
-  <si>
-    <t>Düse,Trommel,Erde,Besteck</t>
-  </si>
-  <si>
-    <t>PRACTICE_ITEMS_EMPH</t>
-  </si>
-  <si>
-    <t>DÜse,TROMmel,ERde,BeSTECK</t>
-  </si>
-  <si>
-    <t>CONTINUE_MAIN_TEST</t>
-  </si>
-  <si>
-    <t>Nun geht der Test los.&lt;br&gt; Viel Vergnügen!</t>
-  </si>
-  <si>
-    <t>Now the test starts.&lt;br&gt; Have fun!</t>
-  </si>
-  <si>
     <t>Beispiel {{page_no}} von {{num_pages}}</t>
   </si>
   <si>
     <t>Example {{page_no}} of {{num_pages}}</t>
   </si>
   <si>
-    <t>EXAMPLE</t>
-  </si>
-  <si>
-    <t>EXAMPLE_PROMPT</t>
-  </si>
-  <si>
-    <t>Hier zunächst ein Beispiel.</t>
-  </si>
-  <si>
-    <t>First, an example.</t>
-  </si>
-  <si>
-    <t>A Sample Question</t>
-  </si>
-  <si>
-    <t>Eine Beispielaufgabe</t>
-  </si>
-  <si>
     <t>Sie haben {{num_correct}} von {{num_items}} Fragen richtig beantwortet ({{perc_correct}}%).</t>
   </si>
   <si>
-    <t>EXAMPLE_FEEDBACK_CORRECT</t>
-  </si>
-  <si>
-    <t>The answer was not correct. Please try again!</t>
-  </si>
-  <si>
-    <t>Das war leider nicht richtig. Versuchen Sie es nochmal!</t>
-  </si>
-  <si>
-    <t>Das war leider zu langsam. Versuchen Sie es nochmal!</t>
-  </si>
-  <si>
-    <t>This was too slow. Please try again!</t>
-  </si>
-  <si>
-    <t>EXAMPLE_FEEDBACK_TOO_SLOW</t>
-  </si>
-  <si>
-    <t>EXAMPLE_FEEDBACK_INCORRECT</t>
-  </si>
-  <si>
     <t>Artist Recognition Test</t>
   </si>
   <si>
@@ -130,21 +64,12 @@
     <t>Literatenquiz</t>
   </si>
   <si>
-    <t>Korrekt.</t>
-  </si>
-  <si>
-    <t>Correct.</t>
-  </si>
-  <si>
     <t>TESTNAME</t>
   </si>
   <si>
     <t>FEEDBACK</t>
   </si>
   <si>
-    <t>You will be presented with a set of name pairs for which you have to decide who is a literary writer (poet, novelist) and who is not.</t>
-  </si>
-  <si>
     <t>Welcome to the Artist Recognition Test!</t>
   </si>
   <si>
@@ -196,13 +121,40 @@
     <t>Welcher der Personen ist eine Literat:in?&lt;br/&gt; Klicken Sie auf den Namen, sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
   </si>
   <si>
-    <t>Sie werden nun mehrere Paare von Namen sehen und müssen jeweils entscheiden, welcher der Persoen eine Literatin (Dichter:in, Schriftsteller:in, Dramatiker:in) ist.</t>
-  </si>
-  <si>
     <t>Is &lt;b&gt;{{name}}&lt;/b&gt; a literary writer? &lt;br/&gt; Click Yes or No, you have {{time_out}} seconds.</t>
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS_SINGLE</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS_SINGLE_PAGE</t>
+  </si>
+  <si>
+    <t>Sie werden eine Liste mit Name sehen und sollen dort ankreuzen, welcher der Personen eine Literat:in (Dichter:in, Schriftsteller:in, Dramatiker:in) ist. Sie haben dazu {{time_out}} Sekunden Zeit.</t>
+  </si>
+  <si>
+    <t>Sie werden nun mehrere Paare von Namen sehen und müssen jeweils entscheiden, welcher der Personen eine Literat:in (Dichter:in, Schriftsteller:in, Dramatiker:in) ist.</t>
+  </si>
+  <si>
+    <t>Sie werden nun Namen präsentiert bekommen und müssen jeweils entscheiden, ob diese Persoen eine Literat:in (Dichter:in, Schriftsteller:in, Dramatiker:in) ist oder nicht.</t>
+  </si>
+  <si>
+    <t>You will be presented with a set of name pairs for which you have to decide who is a literary writer (poet, novelist, playwright) and who is not.</t>
+  </si>
+  <si>
+    <t>INSTRUCTIONS_PAIRS</t>
+  </si>
+  <si>
+    <t>PROMPT_PAIRS</t>
+  </si>
+  <si>
+    <t>You will be presented a set of names for each you will have to decide if it belongs to a literary writer (poet, novelist, playwright) or not.</t>
+  </si>
+  <si>
+    <t>You will be presented with a list of names and you are asked to select all names which belong to a literary writer (poet, novelist, playwright).</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,222 +1026,156 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes as per last spec
</commit_message>
<xml_diff>
--- a/data_raw/dicts/ART_dict.xlsx
+++ b/data_raw/dicts/ART_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B44EF1-7C4B-401C-AE6B-4BDA3EE1DA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E66D8DD-BEB2-457C-93A2-DD8C43D28EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>Sie werden nun mehrere Paare von Namen sehen und müssen jeweils entscheiden, welcher der Personen eine Literat:in (Dichter:in, Schriftsteller:in, Dramatiker:in) ist.</t>
   </si>
   <si>
-    <t>Sie werden nun Namen präsentiert bekommen und müssen jeweils entscheiden, ob diese Persoen eine Literat:in (Dichter:in, Schriftsteller:in, Dramatiker:in) ist oder nicht.</t>
-  </si>
-  <si>
     <t>You will be presented with a set of name pairs for which you have to decide who is a literary writer (poet, novelist, playwright) and who is not.</t>
   </si>
   <si>
@@ -151,10 +148,14 @@
     <t>PROMPT_PAIRS</t>
   </si>
   <si>
-    <t>You will be presented a set of names for each you will have to decide if it belongs to a literary writer (poet, novelist, playwright) or not.</t>
-  </si>
-  <si>
     <t>You will be presented with a list of names and you are asked to select all names which belong to a literary writer (poet, novelist, playwright). You have {{time_out}} seconds to do this.</t>
+  </si>
+  <si>
+    <t>Im Folgenden zeigen wir Ihnen eine Reihe von Personennamen und fragen Sie jeweils, ob es sich bei diesen Personen um literarische Autor*innen handelt, also um Autoren und Autorinnen von literarischer Prosa, Gedichten oder Dramen. Dies trifft nur für einige der gelisteten Namen zu.&lt;br/&gt;
+Bitte klicken Sie nur dann „ja“ an, wenn Sie &lt;strong&gt;sich sicher sind&lt;/strong&gt;, dass es sich um die Namen literarischer Autor*innen handelt. Wenn Sie nicht wissen, ob es sich um eine/n Autor*in handelt, oder wissen, dass es sich nicht um eine/n Autor*in handelt, klicken Sie „nein/weiß nicht“. Bitte raten Sie nicht. Sie haben für jede Antwort &lt;strong&gt;maximal 10 Sekunden Zeit&lt;/strong&gt;. Wenn Sie sich innerhalb dieser Zeit nicht entschieden haben, wird automatisch der nächste Name angezeigt.</t>
+  </si>
+  <si>
+    <t>In the following, we show you a number of personal names and ask you in each case whether these persons are literary authors, i.e. authors of literary prose, poetry or drama. This only applies to some of the names listed.&lt;br/&gt; Please only click "yes" if you are &lt;strong&gt;sure&lt;/strong&gt; that these are the names of literary authors. If you do not know if it is an author or know that it is not an author, click "no/don't know". Please do not guess. You have &lt;strong&gt;a maximum of 10 seconds&lt;/strong&gt; for each answer. If you have not made a decision within this time, the next name will be displayed automatically.</t>
   </si>
 </sst>
 </file>
@@ -1004,12 +1005,12 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1037,13 +1038,13 @@
     </row>
     <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1051,10 +1052,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1065,12 +1066,12 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Small fixes to SLS and ART texts
</commit_message>
<xml_diff>
--- a/data_raw/dicts/ART_dict.xlsx
+++ b/data_raw/dicts/ART_dict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F45DB3-F531-455D-8774-FAC28F5FFAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A72AA24-BBFD-4AD4-85CF-F7E537618E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>PROMPT_SINGLE</t>
   </si>
   <si>
-    <t>Welcher der Personen ist eine Literat:in?&lt;br/&gt; Klicken Sie auf den Namen, sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
-  </si>
-  <si>
     <t>Is &lt;b&gt;{{name}}&lt;/b&gt; a literary writer? &lt;br/&gt; Click Yes or No, you have {{time_out}} seconds.</t>
   </si>
   <si>
@@ -136,12 +133,6 @@
     <t>In the following, we show you a number of personal names and ask you in each case whether these persons are literary authors, i.e. authors of literary prose, poetry or drama. This only applies to some of the names listed.&lt;br/&gt; Please only click "yes" if you are &lt;strong&gt;sure&lt;/strong&gt; that these are the names of literary authors. If you do not know if it is an author or know that it is not an author, click "no/don't know". Please do not guess. You have &lt;strong&gt;a maximum of 10 seconds&lt;/strong&gt; for each answer. If you have not made a decision within this time, the next name will be displayed automatically.</t>
   </si>
   <si>
-    <t>Autor:innenquiz</t>
-  </si>
-  <si>
-    <t>Test: Autor:innenquiz</t>
-  </si>
-  <si>
     <t>Ist &lt;b&gt;{{name}}&lt;/b&gt; ein:e Autor:in?&lt;br/&gt; Klicken Sie Ja oder Nein, sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
   </si>
   <si>
@@ -155,9 +146,6 @@
   </si>
   <si>
     <t>FINISHED</t>
-  </si>
-  <si>
-    <t>&lt;h4&gt;Das Autor:innenquiz ist nun beendet.&lt;/h4&gt; Bitte klicken Sie auf "Weiter", um den nächsten Test zu beginnen.</t>
   </si>
   <si>
     <t>Sie haben {{num_correct}} Autori:nnen aus {{num_items}} Namen richtig erkannt ({{perc_correct}}%, Punkte: {{points}}).</t>
@@ -165,6 +153,18 @@
   <si>
     <t>Im Folgenden zeigen wir Ihnen eine Reihe von Personennamen und fragen Sie jeweils, ob es sich bei diesen Personen um Autoren und Autorinnen von literarischer Prosa, Gedichten oder Dramen handelt. Dies trifft nur für einige der gelisteten Namen zu.&lt;br/&gt;
 Bitte klicken Sie nur dann „ja“ an, wenn Sie &lt;strong&gt;sich sicher sind&lt;/strong&gt;, dass es sich um die Namen literarischer Autor:innen handelt. Wenn Sie **nicht wissen**, ob es sich um eine/n Autor:in handelt, oder wissen, dass es sich nicht um eine/n Autor:in handelt, klicken Sie „nein/weiß nicht“. Bitte raten Sie nicht. &lt;br/&gt;Sie haben für jede Antwort &lt;strong&gt;maximal 10 Sekunden Zeit&lt;/strong&gt;. Wenn Sie sich innerhalb dieser Zeit nicht entschieden haben, wird automatisch der nächste Name angezeigt.</t>
+  </si>
+  <si>
+    <t>Autor:inquiz</t>
+  </si>
+  <si>
+    <t>Welcher der Personen ist eine Autor:in?&lt;br/&gt; Klicken Sie auf den Namen, sie haben {{time_out}} Sekunden Zeit zu antworten.</t>
+  </si>
+  <si>
+    <t>Quiz: Autoren und Autorinnen</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Das Autor:inquiz ist nun beendet.&lt;/h4&gt; Bitte klicken Sie auf "Weiter", um den nächsten Test zu beginnen.</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1014,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1039,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1047,43 +1047,43 @@
     </row>
     <row r="3" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -1094,10 +1094,10 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1127,7 +1127,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -1160,7 +1160,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1182,21 +1182,21 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various small fixes: timer in SRS practice, SLS cross hair, typos.
</commit_message>
<xml_diff>
--- a/data_raw/dicts/ART_dict.xlsx
+++ b/data_raw/dicts/ART_dict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\DOTS\development\packages\mpipoet\data_raw\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A72AA24-BBFD-4AD4-85CF-F7E537618E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3B9E9C-4E68-423E-BCFA-D5E1536C3CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3735" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ART_dict" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
     <t>Quiz: Autoren und Autorinnen</t>
   </si>
   <si>
-    <t>&lt;h4&gt;Das Autor:inquiz ist nun beendet.&lt;/h4&gt; Bitte klicken Sie auf "Weiter", um den nächsten Test zu beginnen.</t>
+    <t>&lt;h4&gt;Das Autor:inquiz ist nun beendet.&lt;/h4&gt; Bitte klicken Sie auf „Weiter", um den nächsten Test zu beginnen.</t>
   </si>
 </sst>
 </file>

</xml_diff>